<commit_message>
refactor-update: clean code structure & add Nguyen's validate code
</commit_message>
<xml_diff>
--- a/data/input/tkb_ai.xlsx
+++ b/data/input/tkb_ai.xlsx
@@ -3889,7 +3889,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0">
+    <sheetView topLeftCell="A242" zoomScale="115" workbookViewId="0">
       <selection activeCell="G47" activeCellId="0" sqref="G47"/>
     </sheetView>
   </sheetViews>
@@ -4144,7 +4144,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -8345,7 +8345,7 @@
       <c r="C225" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D225" s="2" t="s">
+      <c r="D225" s="3" t="s">
         <v>432</v>
       </c>
       <c r="E225" s="2" t="s">
@@ -8465,7 +8465,7 @@
       <c r="C231" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="D231" s="2" t="s">
+      <c r="D231" s="3" t="s">
         <v>439</v>
       </c>
       <c r="E231" s="2" t="s">
@@ -8665,7 +8665,7 @@
       <c r="C241" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="D241" s="2" t="s">
+      <c r="D241" s="3" t="s">
         <v>455</v>
       </c>
       <c r="E241" s="2" t="s">
@@ -8825,7 +8825,7 @@
       <c r="C249" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D249" s="2" t="s">
+      <c r="D249" s="3" t="s">
         <v>466</v>
       </c>
       <c r="E249" s="2" t="s">
@@ -8885,7 +8885,7 @@
       <c r="C252" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D252" s="2" t="s">
+      <c r="D252" s="3" t="s">
         <v>472</v>
       </c>
       <c r="E252" s="2" t="s">
@@ -8925,7 +8925,7 @@
       <c r="C254" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D254" s="2" t="s">
+      <c r="D254" s="3" t="s">
         <v>432</v>
       </c>
       <c r="E254" s="2" t="s">

</xml_diff>